<commit_message>
1DES Organizada chamada 1desfreq.xlsx
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -965,7 +965,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,7 +2749,7 @@
         <v>47</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1DES LIMA Add Aula03
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\1des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitwell\senai2021\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -962,10 +962,10 @@
   <dimension ref="A1:BB42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,7 +1561,7 @@
         <v>47</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>47</v>
@@ -1670,7 +1670,7 @@
         <v>47</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>47</v>
@@ -2325,7 +2325,7 @@
         <v>47</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
1DES SOP Add Aula03
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="51">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>Ordem</t>
+  </si>
+  <si>
+    <t>Vitor Hugo Ramos Silva</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -316,7 +322,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -959,13 +970,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB42"/>
+  <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,6 +1205,9 @@
       <c r="M3" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N3" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1235,6 +1249,9 @@
       <c r="M4" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N4" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1276,6 +1293,9 @@
       <c r="M5" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N5" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1317,6 +1337,9 @@
       <c r="M6" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N6" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1358,6 +1381,9 @@
       <c r="M7" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N7" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1399,7 +1425,9 @@
       <c r="M8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="5"/>
+      <c r="N8" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
@@ -1442,6 +1470,9 @@
       <c r="M9" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N9" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1483,6 +1514,9 @@
       <c r="M10" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N10" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1524,7 +1558,9 @@
       <c r="M11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N11" s="8"/>
+      <c r="N11" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="8"/>
@@ -1606,6 +1642,9 @@
       <c r="M12" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N12" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1645,6 +1684,9 @@
         <v>47</v>
       </c>
       <c r="M13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>47</v>
       </c>
       <c r="P13" s="5"/>
@@ -1721,6 +1763,9 @@
       <c r="M14" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N14" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1762,6 +1807,9 @@
       <c r="M15" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="N15" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1803,8 +1851,11 @@
       <c r="M16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1844,8 +1895,11 @@
       <c r="M17" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1885,8 +1939,11 @@
       <c r="M18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1926,8 +1983,11 @@
       <c r="M19" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1967,8 +2027,11 @@
       <c r="M20" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2008,8 +2071,11 @@
       <c r="M21" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2049,8 +2115,11 @@
       <c r="M22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2090,8 +2159,11 @@
       <c r="M23" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2131,8 +2203,11 @@
       <c r="M24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2172,8 +2247,11 @@
       <c r="M25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2213,8 +2291,11 @@
       <c r="M26" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2254,8 +2335,11 @@
       <c r="M27" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2295,8 +2379,11 @@
       <c r="M28" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2336,8 +2423,11 @@
       <c r="M29" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2377,8 +2467,11 @@
       <c r="M30" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2418,8 +2511,11 @@
       <c r="M31" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2454,13 +2550,16 @@
         <v>47</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2500,8 +2599,11 @@
       <c r="M33" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2541,8 +2643,11 @@
       <c r="M34" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2580,10 +2685,13 @@
         <v>47</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2623,8 +2731,11 @@
       <c r="M36" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2664,8 +2775,11 @@
       <c r="M37" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2705,8 +2819,11 @@
       <c r="M38" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2746,8 +2863,11 @@
       <c r="M39" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2787,8 +2907,11 @@
       <c r="M40" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2828,8 +2951,11 @@
       <c r="M41" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2867,6 +2993,53 @@
         <v>47</v>
       </c>
       <c r="M42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N43" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2875,7 +3048,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="C3:CX90">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
aula do dia 08/03/2021
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitwell\senai2021\1des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\2021\Senai\Matérias\senai2021\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322D2E8E-690C-459D-B0E4-0747E5D939EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos" sheetId="2" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Aluno</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="51">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -241,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,7 +604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -613,18 +614,18 @@
       <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -635,7 +636,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -643,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -651,7 +652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -659,7 +660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -667,7 +668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -675,7 +676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -683,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -691,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -699,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -707,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -715,7 +716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -723,7 +724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -731,7 +732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -739,7 +740,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -747,7 +748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -755,7 +756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -763,7 +764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -771,7 +772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -779,7 +780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -787,7 +788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -795,7 +796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -803,7 +804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -811,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -819,7 +820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -827,7 +828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -835,7 +836,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -843,7 +844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -851,7 +852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -859,7 +860,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -867,7 +868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -875,7 +876,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -883,7 +884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -891,7 +892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -899,7 +900,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -907,7 +908,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -915,7 +916,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -923,7 +924,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -931,7 +932,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -939,7 +940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -947,7 +948,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -956,7 +957,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:C42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C42">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -964,25 +965,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="29" width="7" style="2" customWidth="1"/>
-    <col min="30" max="54" width="9.140625" style="2"/>
+    <col min="30" max="54" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1160,7 +1161,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1206,8 +1207,11 @@
       <c r="O3" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1253,8 +1257,11 @@
       <c r="O4" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1300,8 +1307,11 @@
       <c r="O5" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1347,8 +1357,11 @@
       <c r="O6" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1394,8 +1407,11 @@
       <c r="O7" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P7" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1442,7 +1458,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1488,8 +1504,11 @@
       <c r="O9" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1535,8 +1554,11 @@
       <c r="O10" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1582,7 +1604,9 @@
       <c r="O11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="P11" s="8"/>
+      <c r="P11" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
@@ -1622,7 +1646,7 @@
       <c r="BA11" s="8"/>
       <c r="BB11" s="8"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1668,8 +1692,11 @@
       <c r="O12" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P12" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1715,7 +1742,9 @@
       <c r="O13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
@@ -1749,7 +1778,7 @@
       <c r="AU13" s="5"/>
       <c r="AV13" s="5"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1795,8 +1824,11 @@
       <c r="O14" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1842,8 +1874,11 @@
       <c r="O15" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="P15" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1889,8 +1924,11 @@
       <c r="O16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1936,8 +1974,11 @@
       <c r="O17" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1983,8 +2024,11 @@
       <c r="O18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2030,8 +2074,11 @@
       <c r="O19" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2077,8 +2124,11 @@
       <c r="O20" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2124,8 +2174,11 @@
       <c r="O21" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2171,8 +2224,11 @@
       <c r="O22" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2218,8 +2274,11 @@
       <c r="O23" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2265,8 +2324,11 @@
       <c r="O24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2312,8 +2374,11 @@
       <c r="O25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2359,8 +2424,11 @@
       <c r="O26" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2406,8 +2474,11 @@
       <c r="O27" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2453,8 +2524,11 @@
       <c r="O28" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2500,8 +2574,11 @@
       <c r="O29" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2547,8 +2624,11 @@
       <c r="O30" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2594,8 +2674,11 @@
       <c r="O31" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2641,8 +2724,11 @@
       <c r="O32" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2688,8 +2774,11 @@
       <c r="O33" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2735,8 +2824,11 @@
       <c r="O34" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -2782,8 +2874,11 @@
       <c r="O35" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -2829,8 +2924,11 @@
       <c r="O36" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2876,8 +2974,11 @@
       <c r="O37" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2923,8 +3024,11 @@
       <c r="O38" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2970,8 +3074,11 @@
       <c r="O39" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -3017,8 +3124,11 @@
       <c r="O40" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3064,8 +3174,11 @@
       <c r="O41" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -3111,8 +3224,11 @@
       <c r="O42" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3158,9 +3274,12 @@
       <c r="O43" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="P43" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A3:O42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O42">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="C3:CX90">

</xml_diff>

<commit_message>
aula de HARE 12/03
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\1des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\2021\Senai\Matérias\senai2021\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3745D1-9DC1-4E26-A9D7-ECDF1213E41F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos" sheetId="2" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Aluno</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="51">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -241,7 +242,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -322,7 +323,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -603,28 +609,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -635,7 +641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -643,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -651,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -662,7 +668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -670,7 +676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -678,7 +684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -686,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -694,7 +700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -702,7 +708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -710,7 +716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -718,7 +724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -726,7 +732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -734,7 +740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -745,7 +751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -753,7 +759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -764,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -775,7 +781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -783,7 +789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -791,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -799,7 +805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -807,7 +813,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -815,7 +821,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -823,7 +829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -831,7 +837,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -839,7 +845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -847,7 +853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -855,7 +861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -863,7 +869,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -871,7 +877,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -879,7 +885,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -887,7 +893,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -895,7 +901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -906,7 +912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -914,7 +920,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -922,7 +928,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -930,7 +936,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -941,7 +947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -949,7 +955,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -960,7 +966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -968,7 +974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -980,7 +986,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:C42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C42">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -989,25 +995,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="29" width="7" style="2" customWidth="1"/>
-    <col min="30" max="54" width="9.140625" style="2"/>
+    <col min="30" max="54" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1093,7 +1099,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1240,8 +1246,14 @@
       <c r="R3" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1296,8 +1308,14 @@
       <c r="R4" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1352,8 +1370,14 @@
       <c r="R5" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1408,8 +1432,14 @@
       <c r="R6" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1464,8 +1494,14 @@
       <c r="R7" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1512,7 +1548,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1567,8 +1603,14 @@
       <c r="R9" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1623,8 +1665,14 @@
       <c r="R10" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1679,8 +1727,12 @@
       <c r="R11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
+      <c r="S11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
@@ -1716,7 +1768,7 @@
       <c r="BA11" s="8"/>
       <c r="BB11" s="8"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1771,8 +1823,14 @@
       <c r="R12" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1827,8 +1885,12 @@
       <c r="R13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
+      <c r="S13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
@@ -1858,7 +1920,7 @@
       <c r="AU13" s="5"/>
       <c r="AV13" s="5"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1913,8 +1975,14 @@
       <c r="R14" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1969,8 +2037,14 @@
       <c r="R15" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="S15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2025,8 +2099,14 @@
       <c r="R16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2081,8 +2161,14 @@
       <c r="R17" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2137,8 +2223,14 @@
       <c r="R18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2193,8 +2285,14 @@
       <c r="R19" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2249,8 +2347,14 @@
       <c r="R20" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2305,8 +2409,14 @@
       <c r="R21" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2361,8 +2471,14 @@
       <c r="R22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2417,8 +2533,14 @@
       <c r="R23" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2473,8 +2595,14 @@
       <c r="R24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2529,8 +2657,14 @@
       <c r="R25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2585,8 +2719,14 @@
       <c r="R26" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2641,8 +2781,14 @@
       <c r="R27" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2697,8 +2843,14 @@
       <c r="R28" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2753,8 +2905,14 @@
       <c r="R29" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T29" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2809,8 +2967,14 @@
       <c r="R30" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2865,8 +3029,14 @@
       <c r="R31" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2921,8 +3091,14 @@
       <c r="R32" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T32" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2977,8 +3153,14 @@
       <c r="R33" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -3033,8 +3215,14 @@
       <c r="R34" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -3089,8 +3277,14 @@
       <c r="R35" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -3145,8 +3339,14 @@
       <c r="R36" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T36" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -3201,8 +3401,14 @@
       <c r="R37" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3257,8 +3463,14 @@
       <c r="R38" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T38" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -3313,8 +3525,14 @@
       <c r="R39" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -3369,8 +3587,14 @@
       <c r="R40" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3425,8 +3649,14 @@
       <c r="R41" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T41" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -3481,8 +3711,14 @@
       <c r="R42" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3537,12 +3773,23 @@
       <c r="R43" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T43" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A3:O42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:O42">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="C3:CX90">
+  <conditionalFormatting sqref="C44:CX90 C3:R43 T3:CX43">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S43">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>

</xml_diff>

<commit_message>
1DES SOP aula05 word
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\2021\Senai\Matérias\senai2021\1des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\users\desktpop\github\senai2021\1des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3745D1-9DC1-4E26-A9D7-ECDF1213E41F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087FB0E8-E1C8-4B08-A4A7-DF4BE723ECF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos" sheetId="2" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="52">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Orçamento</t>
   </si>
 </sst>
 </file>
@@ -610,27 +613,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -640,8 +647,11 @@
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -649,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -657,7 +667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -668,7 +678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -676,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -684,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -692,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -700,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -708,7 +718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -716,7 +726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -724,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -732,7 +742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -740,7 +750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -751,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -759,7 +769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -770,7 +780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -781,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -789,7 +799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -797,7 +807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -805,7 +815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -813,7 +823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -821,7 +831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -829,7 +839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -837,7 +847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -845,7 +855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -853,7 +863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -861,7 +871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -869,7 +879,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -877,7 +887,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -885,7 +895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -893,7 +903,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -901,7 +911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -912,7 +922,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -920,7 +930,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -928,7 +938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -936,7 +946,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -947,7 +957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -955,7 +965,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -966,7 +976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -974,7 +984,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -998,22 +1008,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BB43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="29" width="7" style="2" customWidth="1"/>
-    <col min="30" max="54" width="9.109375" style="2"/>
+    <col min="30" max="54" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1109,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1191,7 +1201,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1263,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1315,7 +1325,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1377,7 +1387,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1439,7 +1449,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1501,7 +1511,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1548,7 +1558,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1610,7 +1620,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1672,7 +1682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1768,7 +1778,7 @@
       <c r="BA11" s="8"/>
       <c r="BB11" s="8"/>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1830,7 +1840,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1920,7 +1930,7 @@
       <c r="AU13" s="5"/>
       <c r="AV13" s="5"/>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1982,7 +1992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2044,7 +2054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2106,7 +2116,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2178,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2230,7 +2240,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2292,7 +2302,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2354,7 +2364,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2416,7 +2426,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2478,7 +2488,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2540,7 +2550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2602,7 +2612,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2664,7 +2674,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2726,7 +2736,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2788,7 +2798,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2850,7 +2860,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2912,7 +2922,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2974,7 +2984,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -3036,7 +3046,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -3098,7 +3108,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3160,7 +3170,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -3222,7 +3232,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -3284,7 +3294,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -3346,7 +3356,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -3408,7 +3418,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3470,7 +3480,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -3532,7 +3542,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -3594,7 +3604,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3656,7 +3666,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -3718,7 +3728,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
3DES projetos grupo restaurante
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="51">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -322,7 +322,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -606,11 +611,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,11 +997,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,6 +1245,9 @@
       <c r="R3" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S3" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1296,6 +1304,9 @@
       <c r="R4" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S4" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1352,6 +1363,9 @@
       <c r="R5" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1408,6 +1422,9 @@
       <c r="R6" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S6" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1464,6 +1481,9 @@
       <c r="R7" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S7" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1567,6 +1587,9 @@
       <c r="R9" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1623,6 +1646,9 @@
       <c r="R10" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S10" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1679,7 +1705,9 @@
       <c r="R11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="S11" s="8"/>
+      <c r="S11" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="T11" s="8"/>
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
@@ -1771,6 +1799,9 @@
       <c r="R12" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S12" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1818,16 +1849,18 @@
       <c r="O13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="P13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="R13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="S13" s="5"/>
+      <c r="P13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
       <c r="V13" s="5"/>
@@ -1913,6 +1946,9 @@
       <c r="R14" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S14" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1969,6 +2005,9 @@
       <c r="R15" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="S15" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2025,8 +2064,11 @@
       <c r="R16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2081,8 +2123,11 @@
       <c r="R17" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2137,8 +2182,11 @@
       <c r="R18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2193,8 +2241,11 @@
       <c r="R19" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2249,8 +2300,11 @@
       <c r="R20" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2305,8 +2359,11 @@
       <c r="R21" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2361,8 +2418,11 @@
       <c r="R22" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2417,8 +2477,11 @@
       <c r="R23" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -2473,8 +2536,11 @@
       <c r="R24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2529,8 +2595,11 @@
       <c r="R25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -2585,8 +2654,11 @@
       <c r="R26" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2641,8 +2713,11 @@
       <c r="R27" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2697,8 +2772,11 @@
       <c r="R28" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -2753,8 +2831,11 @@
       <c r="R29" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -2809,8 +2890,11 @@
       <c r="R30" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
@@ -2865,8 +2949,11 @@
       <c r="R31" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -2921,8 +3008,11 @@
       <c r="R32" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2977,8 +3067,11 @@
       <c r="R33" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -3033,8 +3126,11 @@
       <c r="R34" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -3089,8 +3185,11 @@
       <c r="R35" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -3145,8 +3244,11 @@
       <c r="R36" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -3201,8 +3303,11 @@
       <c r="R37" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -3257,8 +3362,11 @@
       <c r="R38" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -3313,8 +3421,11 @@
       <c r="R39" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -3369,8 +3480,11 @@
       <c r="R40" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -3425,8 +3539,11 @@
       <c r="R41" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -3481,8 +3598,11 @@
       <c r="R42" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3535,6 +3655,9 @@
         <v>47</v>
       </c>
       <c r="R43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S43" s="2" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3543,7 +3666,7 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="C3:CX90">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Notas de SOP adicionadas
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos" sheetId="2" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="53">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -236,13 +236,19 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Somativa</t>
+  </si>
+  <si>
+    <t>Orçamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,6 +285,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -300,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -318,16 +332,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -609,27 +619,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -639,24 +659,39 @@
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -666,64 +701,82 @@
       <c r="C5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -731,15 +784,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -749,16 +802,22 @@
       <c r="C15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -768,8 +827,11 @@
       <c r="C17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -779,128 +841,174 @@
       <c r="C18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F18" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F32" s="7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -910,32 +1018,44 @@
       <c r="C34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F35" s="7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F36" s="7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>15</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -945,16 +1065,22 @@
       <c r="C38" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -964,16 +1090,22 @@
       <c r="C40">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -982,6 +1114,20 @@
       </c>
       <c r="C42">
         <v>8</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="F43">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -995,24 +1141,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB43"/>
+  <dimension ref="A1:AO43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S3" sqref="S3"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="29" width="7" style="2" customWidth="1"/>
-    <col min="30" max="54" width="9.140625" style="2"/>
+    <col min="3" max="19" width="7" style="2" customWidth="1"/>
+    <col min="20" max="41" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1064,41 +1210,8 @@
       <c r="S1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1156,41 +1269,8 @@
       <c r="S2" s="3">
         <v>44266</v>
       </c>
-      <c r="T2" s="3">
-        <v>44267</v>
-      </c>
-      <c r="U2" s="3">
-        <v>44270</v>
-      </c>
-      <c r="V2" s="3">
-        <v>44271</v>
-      </c>
-      <c r="W2" s="3">
-        <v>44272</v>
-      </c>
-      <c r="X2" s="3">
-        <v>44273</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>44274</v>
-      </c>
-      <c r="Z2" s="3">
-        <v>44277</v>
-      </c>
-      <c r="AA2" s="3">
-        <v>44278</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>44279</v>
-      </c>
-      <c r="AC2" s="3">
-        <v>44280</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>44281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1249,7 +1329,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1308,7 +1388,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1367,7 +1447,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1426,7 +1506,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1485,7 +1565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1532,7 +1612,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1591,7 +1671,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1650,7 +1730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:54" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>28</v>
       </c>
@@ -1730,21 +1810,8 @@
       <c r="AM11" s="8"/>
       <c r="AN11" s="8"/>
       <c r="AO11" s="8"/>
-      <c r="AP11" s="8"/>
-      <c r="AQ11" s="8"/>
-      <c r="AR11" s="8"/>
-      <c r="AS11" s="8"/>
-      <c r="AT11" s="8"/>
-      <c r="AU11" s="8"/>
-      <c r="AV11" s="8"/>
-      <c r="AW11" s="8"/>
-      <c r="AX11" s="8"/>
-      <c r="AY11" s="8"/>
-      <c r="AZ11" s="8"/>
-      <c r="BA11" s="8"/>
-      <c r="BB11" s="8"/>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1803,7 +1870,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1877,21 +1944,8 @@
       <c r="AG13" s="5"/>
       <c r="AH13" s="5"/>
       <c r="AI13" s="5"/>
-      <c r="AJ13" s="5"/>
-      <c r="AK13" s="5"/>
-      <c r="AL13" s="5"/>
-      <c r="AM13" s="5"/>
-      <c r="AN13" s="5"/>
-      <c r="AO13" s="5"/>
-      <c r="AP13" s="5"/>
-      <c r="AQ13" s="5"/>
-      <c r="AR13" s="5"/>
-      <c r="AS13" s="5"/>
-      <c r="AT13" s="5"/>
-      <c r="AU13" s="5"/>
-      <c r="AV13" s="5"/>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1950,7 +2004,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2009,7 +2063,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -3665,8 +3719,8 @@
   <sortState ref="A3:O42">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="C3:CX90">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="C3:CK90">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
3DES add aula21 e 22
</commit_message>
<xml_diff>
--- a/1des/1desfreq.xlsx
+++ b/1des/1desfreq.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="56">
   <si>
     <t>Gabriel Vital Ferreira</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t>Orçamento</t>
+  </si>
+  <si>
+    <t>Analizando</t>
+  </si>
+  <si>
+    <t>Evadiu</t>
+  </si>
+  <si>
+    <t>Ausente</t>
   </si>
 </sst>
 </file>
@@ -619,13 +628,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,9 +642,10 @@
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>41</v>
       </c>
@@ -649,7 +659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -669,7 +679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -680,7 +690,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -691,7 +701,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -705,7 +715,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -716,7 +726,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -727,15 +737,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -746,7 +759,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -757,15 +770,18 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -776,23 +792,29 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -806,7 +828,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -817,7 +839,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -831,7 +853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -845,7 +867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -856,7 +878,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -867,7 +889,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -878,7 +900,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -889,7 +911,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -900,7 +922,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -908,8 +930,11 @@
         <v>23</v>
       </c>
       <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -920,7 +945,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -931,7 +956,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -942,7 +967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -953,7 +978,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -964,7 +989,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -975,7 +1000,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -986,7 +1011,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>

</xml_diff>